<commit_message>
add manufacture analysis in the README
</commit_message>
<xml_diff>
--- a/data/for_tableau/vaccination_manu.xlsx
+++ b/data/for_tableau/vaccination_manu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\job\project\COVID-19-Vaccination-Data-Visualization\data\for_tableau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99AB9D4-3E3D-4C81-8714-99877F15CC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93B34AB-30E8-4674-A554-A540FB8FDACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{B96CD49C-7920-4C90-B1E4-0C0DC363DD7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B96CD49C-7920-4C90-B1E4-0C0DC363DD7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -525,11 +525,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C88750-3575-44EE-9074-D3CF499D70D6}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1063,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D311A8-D01A-4572-8FCB-06614D8D6FEB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>